<commit_message>
add more info on cultivars
</commit_message>
<xml_diff>
--- a/manuscript/Figures_&_tables/Supplementary Table 1 Cultivars.xlsx
+++ b/manuscript/Figures_&_tables/Supplementary Table 1 Cultivars.xlsx
@@ -1,30 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\montazeaud\Documents\RECHERCHE\Postdoc\Montpellier\SolACE 3\SolACE_wheat_mixtures\manuscript\Figures_&amp;_tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/freville/MyFiles/Articles/En_cours/Mixtures_4PMI_SolACE/Figures_&amp;_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60158D8-AC76-6C41-8F7A-6F91FCE0BAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="7908"/>
+    <workbookView xWindow="8100" yWindow="500" windowWidth="35920" windowHeight="26460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$C$37</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="46">
   <si>
     <t>Genotype</t>
   </si>
@@ -137,22 +151,37 @@
     <t>SVEVO</t>
   </si>
   <si>
-    <t>Breeding company/Research Institute</t>
-  </si>
-  <si>
     <t>INRAE Montpellier</t>
   </si>
   <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Country</t>
+    <t>Panel</t>
+  </si>
+  <si>
+    <t>UNIBO</t>
+  </si>
+  <si>
+    <t>CREA</t>
+  </si>
+  <si>
+    <t>GPDUR</t>
+  </si>
+  <si>
+    <t>EPO</t>
+  </si>
+  <si>
+    <t>Bologna University</t>
+  </si>
+  <si>
+    <t>Collection</t>
+  </si>
+  <si>
+    <t>Arvalis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -472,245 +501,425 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="190" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
-    <col min="3" max="3" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>